<commit_message>
feat: Add table generation modules for game data processing
- Implemented modules for generating various tables from merged master data:
  - media_tables: Handles images and videos.
  - support_tables: Manages support information.
  - requirements_tables: Extracts system requirements.
  - platforms_tables: Captures operating system compatibility.
  - package_tables: Processes packages and sub-packages.
  - developer_publisher_tables: Generates developer and publisher data.
  - genre_category_tables: Creates genre and category tables.
  - tags_tables: Manages tags associated with games.
  - game_metadata: Extracts game descriptions and metadata.
  - language_tables: Handles supported languages.

- Added utility functions for file handling and text processing.
- Enhanced logging for better traceability of data processing.
</commit_message>
<xml_diff>
--- a/doc/Dictionaries/A_schema_data_dictionary.xlsx
+++ b/doc/Dictionaries/A_schema_data_dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zalma\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zalma\videogame-data-analysis\doc\Dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6F5801-5557-4D52-9B31-3D02D7BB7787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1D1BE4-90B8-49AA-ABDC-C0CF4B489405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,24 +21,37 @@
     <sheet name="movies" sheetId="6" r:id="rId6"/>
     <sheet name="requirements" sheetId="7" r:id="rId7"/>
     <sheet name="tags" sheetId="8" r:id="rId8"/>
-    <sheet name="genres" sheetId="9" r:id="rId9"/>
-    <sheet name="platforms" sheetId="10" r:id="rId10"/>
-    <sheet name="categories" sheetId="11" r:id="rId11"/>
-    <sheet name="publishers" sheetId="12" r:id="rId12"/>
-    <sheet name="developers" sheetId="13" r:id="rId13"/>
-    <sheet name="game_tag" sheetId="14" r:id="rId14"/>
-    <sheet name="game_genre" sheetId="15" r:id="rId15"/>
-    <sheet name="game_platform" sheetId="16" r:id="rId16"/>
-    <sheet name="game_category" sheetId="17" r:id="rId17"/>
-    <sheet name="game_publisher" sheetId="18" r:id="rId18"/>
+    <sheet name="game_tag" sheetId="14" r:id="rId9"/>
+    <sheet name="genres" sheetId="9" r:id="rId10"/>
+    <sheet name="game_genre" sheetId="15" r:id="rId11"/>
+    <sheet name="platforms" sheetId="10" r:id="rId12"/>
+    <sheet name="game_platform" sheetId="16" r:id="rId13"/>
+    <sheet name="categories" sheetId="11" r:id="rId14"/>
+    <sheet name="game_category" sheetId="17" r:id="rId15"/>
+    <sheet name="publishers" sheetId="12" r:id="rId16"/>
+    <sheet name="game_publisher" sheetId="18" r:id="rId17"/>
+    <sheet name="developers" sheetId="13" r:id="rId18"/>
     <sheet name="game_developer" sheetId="19" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="84">
   <si>
     <t>Oszlop</t>
   </si>
@@ -100,9 +113,6 @@
     <t>required_age</t>
   </si>
   <si>
-    <t>achievements</t>
-  </si>
-  <si>
     <t>&gt;=0</t>
   </si>
   <si>
@@ -220,9 +230,6 @@
     <t>{minimum, recommended}</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>max 2000</t>
   </si>
   <si>
@@ -281,6 +288,21 @@
   </si>
   <si>
     <t>&gt;=1997-06-30 és &lt;=2019-05-01</t>
+  </si>
+  <si>
+    <t>requirements</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>≥ 0</t>
+  </si>
+  <si>
+    <t>A-Za-z0-9\s\-\++$</t>
+  </si>
+  <si>
+    <t>num_achievements</t>
   </si>
 </sst>
 </file>
@@ -643,15 +665,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
@@ -707,7 +729,7 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -715,16 +737,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -735,90 +757,104 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
+      <c r="D7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -827,190 +863,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
@@ -1032,7 +894,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1046,16 +908,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1063,64 +925,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1151,18 +962,18 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1170,11 +981,74 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="A1:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1205,18 +1079,18 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1224,11 +1098,74 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1260,18 +1197,18 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1279,11 +1216,74 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1315,18 +1315,18 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1334,11 +1334,75 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1370,18 +1434,18 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1391,9 +1455,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1419,7 +1485,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1439,49 +1505,35 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
         <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1494,7 +1546,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="A2" sqref="A2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,7 +1573,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1541,18 +1593,18 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -1560,13 +1612,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -1574,13 +1626,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1595,7 +1647,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1621,7 +1675,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1641,35 +1695,35 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1681,7 +1735,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1707,7 +1763,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1727,21 +1783,21 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1753,7 +1809,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1778,7 +1836,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1798,21 +1856,21 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1824,11 +1882,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
@@ -1850,7 +1910,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1870,46 +1930,46 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
         <v>56</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1922,9 +1982,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1949,7 +2011,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1963,16 +2025,27 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1981,17 +2054,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2010,30 +2083,24 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>